<commit_message>
environment works but is organized shit
</commit_message>
<xml_diff>
--- a/qasm_analysis_3_trap_transfer.xlsx
+++ b/qasm_analysis_3_trap_transfer.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,401 +473,26 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ising_n98_transpiled.qasm</t>
+          <t>google_advantage.qasm</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.01608704277522737</v>
+        <v>0.7982613480018267</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01608704277522737</v>
+        <v>0.7945860629791764</v>
       </c>
       <c r="D2" t="n">
-        <v>99</v>
+        <v>28</v>
       </c>
       <c r="E2" t="n">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="F2" t="n">
-        <v>187</v>
+        <v>32</v>
       </c>
       <c r="G2" t="n">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>qaoa_circuit_20_4.qasm</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0.4504501307805319</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.4504501307805319</v>
-      </c>
-      <c r="D3" t="n">
-        <v>55</v>
-      </c>
-      <c r="E3" t="n">
-        <v>55</v>
-      </c>
-      <c r="F3" t="n">
-        <v>76</v>
-      </c>
-      <c r="G3" t="n">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ising_n26.qasm</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0.599326575232672</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.599326575232672</v>
-      </c>
-      <c r="D4" t="n">
-        <v>27</v>
-      </c>
-      <c r="E4" t="n">
-        <v>27</v>
-      </c>
-      <c r="F4" t="n">
-        <v>49</v>
-      </c>
-      <c r="G4" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>dnn_n51_transpiled.qasm</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.003659274240275831</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.002797244170942612</v>
-      </c>
-      <c r="D5" t="n">
-        <v>269</v>
-      </c>
-      <c r="E5" t="n">
-        <v>252</v>
-      </c>
-      <c r="F5" t="n">
-        <v>271</v>
-      </c>
-      <c r="G5" t="n">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>vqe_n4_transpiled.qasm</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.9391719980261437</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.9391719980261437</v>
-      </c>
-      <c r="D6" t="n">
-        <v>7</v>
-      </c>
-      <c r="E6" t="n">
-        <v>7</v>
-      </c>
-      <c r="F6" t="n">
-        <v>9</v>
-      </c>
-      <c r="G6" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>sqrt18.qasm</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>3.829878473929803e-05</v>
-      </c>
-      <c r="C7" t="n">
-        <v>3.030098235237177e-05</v>
-      </c>
-      <c r="D7" t="n">
-        <v>898</v>
-      </c>
-      <c r="E7" t="n">
-        <v>856</v>
-      </c>
-      <c r="F7" t="n">
-        <v>898</v>
-      </c>
-      <c r="G7" t="n">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>dnn_n33_transpiled.qasm</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.0707183695196887</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.06255269054031519</v>
-      </c>
-      <c r="D8" t="n">
-        <v>170</v>
-      </c>
-      <c r="E8" t="n">
-        <v>158</v>
-      </c>
-      <c r="F8" t="n">
-        <v>172</v>
-      </c>
-      <c r="G8" t="n">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>qft_n18.qasm</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0.03262570547925792</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.02984051258584217</v>
-      </c>
-      <c r="D9" t="n">
-        <v>300</v>
-      </c>
-      <c r="E9" t="n">
-        <v>284</v>
-      </c>
-      <c r="F9" t="n">
-        <v>306</v>
-      </c>
-      <c r="G9" t="n">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>DNN16.qasm</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>0.3269407760033544</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.3102413784182018</v>
-      </c>
-      <c r="D10" t="n">
-        <v>87</v>
-      </c>
-      <c r="E10" t="n">
-        <v>74</v>
-      </c>
-      <c r="F10" t="n">
-        <v>125</v>
-      </c>
-      <c r="G10" t="n">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>QV_32.qasm</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1.302193996108339e-10</v>
-      </c>
-      <c r="C11" t="n">
-        <v>7.738876542690178e-11</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1447</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1403</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1488</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1473</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>qaoa_circuit_40_8.qasm</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0.010418072253105</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.010418072253105</v>
-      </c>
-      <c r="D12" t="n">
-        <v>217</v>
-      </c>
-      <c r="E12" t="n">
-        <v>217</v>
-      </c>
-      <c r="F12" t="n">
-        <v>312</v>
-      </c>
-      <c r="G12" t="n">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>hhl_n7.qasm</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0.507471706605126</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.5004452583181059</v>
-      </c>
-      <c r="D13" t="n">
-        <v>90</v>
-      </c>
-      <c r="E13" t="n">
-        <v>81</v>
-      </c>
-      <c r="F13" t="n">
-        <v>92</v>
-      </c>
-      <c r="G13" t="n">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>qaoa_n6_transpiled.qasm</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0.7688953153587761</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.7589543307708074</v>
-      </c>
-      <c r="D14" t="n">
-        <v>32</v>
-      </c>
-      <c r="E14" t="n">
-        <v>25</v>
-      </c>
-      <c r="F14" t="n">
-        <v>36</v>
-      </c>
-      <c r="G14" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>google_advantage.qasm</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>0.7676979607076297</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.7652295892236318</v>
-      </c>
-      <c r="D15" t="n">
-        <v>28</v>
-      </c>
-      <c r="E15" t="n">
-        <v>27</v>
-      </c>
-      <c r="F15" t="n">
-        <v>32</v>
-      </c>
-      <c r="G15" t="n">
         <v>31</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>dder_n10_transpiled.qasm</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.6266129947137067</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.6250617265957956</v>
-      </c>
-      <c r="D16" t="n">
-        <v>64</v>
-      </c>
-      <c r="E16" t="n">
-        <v>62</v>
-      </c>
-      <c r="F16" t="n">
-        <v>65</v>
-      </c>
-      <c r="G16" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>ising_n34_transpiled.qasm</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>0.4686914267282534</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.4686914267282534</v>
-      </c>
-      <c r="D17" t="n">
-        <v>36</v>
-      </c>
-      <c r="E17" t="n">
-        <v>36</v>
-      </c>
-      <c r="F17" t="n">
-        <v>63</v>
-      </c>
-      <c r="G17" t="n">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>